<commit_message>
Enhance test framework with new utilities and features
- Added dynamic browser handling in `BaseTest.cs` with `CreateBrowserAndPage` method.
- Enabled parallel test execution and data-driven testing in `FindNewCarsTest.cs` using `TestCaseSource` and Excel integration.
- Introduced `DataUtil` for reading test data from Excel files.
- Added `DBManager` for MySQL database connection and query execution.
- Implemented `KeyWordDriven` class for keyword-driven testing.
- Added `MailSender` utility for sending emails with attachments.
- Introduced `XMLLocatorReader` for managing locators via XML files.
- Updated `TestSpreadSheet.xlsx` with new test data (binary changes).
- Improved framework flexibility, scalability, and maintainability.
</commit_message>
<xml_diff>
--- a/resources/TestSpreadSheet.xlsx
+++ b/resources/TestSpreadSheet.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\woodr\source\repos\playwright\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\woodr\source\repos\PageObjectModelPW\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{552AD6BD-18DE-4ADB-80D6-B6BC3150A213}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{379307E2-B41A-4BF2-B2EC-E7BC00F217C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{B0960BCF-52F0-4C8D-81B4-BE3083B9D9A2}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{B0960BCF-52F0-4C8D-81B4-BE3083B9D9A2}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginTest" sheetId="1" r:id="rId1"/>
-    <sheet name="UserRegTest" sheetId="2" r:id="rId2"/>
+    <sheet name="FindCarTest" sheetId="3" r:id="rId2"/>
+    <sheet name="UserRegTest" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
   <si>
     <t>username</t>
   </si>
@@ -103,6 +104,36 @@
   </si>
   <si>
     <t>LastTest</t>
+  </si>
+  <si>
+    <t>carbrand</t>
+  </si>
+  <si>
+    <t>browserType</t>
+  </si>
+  <si>
+    <t>runmode</t>
+  </si>
+  <si>
+    <t>chrome</t>
+  </si>
+  <si>
+    <t>firefox</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>bmw</t>
+  </si>
+  <si>
+    <t>mg</t>
+  </si>
+  <si>
+    <t>toyota</t>
   </si>
 </sst>
 </file>
@@ -544,10 +575,72 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D1C5FD9-9A2A-48E1-96F7-871DE345E001}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="14" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C10F850C-437A-4316-93AA-6E12EDEC51B3}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Upgrade dependencies and enhance test framework
Upgraded NuGet packages in `PageObjectModelPW.csproj` to newer versions, including `EPPlus`, `log4net`, `Microsoft.Playwright`, and others. Added `reports` and `screenshots` folders to the project structure.

Refactored `BaseTest.cs` to improve test reporting with `ExtentReports`, ensure proper directory creation, and validate test site URL configuration. Updated `BeforeEachTest` to use `async Task` and improved browser navigation logic.

Modified `NewCarsPage.cs` to update the locator for "MG" to "Maruti Suzuki Cars". Enhanced `FindNewCarsTest.cs` to handle additional car brands like `Toyota`.

Improved `DataUtil.cs` to enforce EPPlus licensing, normalize column handling, skip rows with "runmode=N", and add diagnostic logging for debugging.

Updated `TestSpreadSheet.xlsx` (binary changes not detailed).
</commit_message>
<xml_diff>
--- a/resources/TestSpreadSheet.xlsx
+++ b/resources/TestSpreadSheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\woodr\source\repos\PageObjectModelPW\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{379307E2-B41A-4BF2-B2EC-E7BC00F217C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09A2F92C-68E5-4A8A-A7FF-B945B718AEB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{B0960BCF-52F0-4C8D-81B4-BE3083B9D9A2}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="30">
   <si>
     <t>username</t>
   </si>
@@ -118,13 +118,7 @@
     <t>chrome</t>
   </si>
   <si>
-    <t>firefox</t>
-  </si>
-  <si>
     <t>Y</t>
-  </si>
-  <si>
-    <t>N</t>
   </si>
   <si>
     <t>bmw</t>
@@ -579,7 +573,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -600,35 +594,35 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B2" t="s">
         <v>25</v>
       </c>
       <c r="C2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" t="s">
         <v>26</v>
-      </c>
-      <c r="C3" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B4" t="s">
         <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactor test logic and enhance Excel data handling
Refactored `FindNewCarsTest.cs` to replace `if-else` conditions with a `Dictionary` for car brand navigation, improving readability and maintainability. Added proper exception handling and resource cleanup with a `try-catch-finally` block. Introduced fallback for unsupported car brands and added logging for better debugging.

Enhanced `DataUtil.cs` to improve Excel data handling by simplifying column matching, adding diagnostic logging, and streamlining test data extraction. Implemented a mechanism to mark test cases as ignored when `runmode` is `N`, improving test visibility. Improved error handling and test case naming for better traceability.

Cleaned up redundant code, updated the `DataUtil` constructor for clarity, and ensured compliance with `ExcelPackage` licensing requirements.
</commit_message>
<xml_diff>
--- a/resources/TestSpreadSheet.xlsx
+++ b/resources/TestSpreadSheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\woodr\source\repos\PageObjectModelPW\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09A2F92C-68E5-4A8A-A7FF-B945B718AEB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3741B049-5E43-432E-B397-5598FB4E83BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{B0960BCF-52F0-4C8D-81B4-BE3083B9D9A2}"/>
   </bookViews>
@@ -118,9 +118,6 @@
     <t>chrome</t>
   </si>
   <si>
-    <t>Y</t>
-  </si>
-  <si>
     <t>bmw</t>
   </si>
   <si>
@@ -128,6 +125,9 @@
   </si>
   <si>
     <t>toyota</t>
+  </si>
+  <si>
+    <t>y</t>
   </si>
 </sst>
 </file>
@@ -573,7 +573,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -594,35 +594,35 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B2" t="s">
         <v>25</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B3" t="s">
         <v>25</v>
       </c>
       <c r="C3" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B4" t="s">
         <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Enhance car title validation and refactor framework
- Added `CarBase` class to encapsulate car-related operations.
- Introduced `carBase` static field in `BasePage` for reuse.
- Updated `FindCarTest` to validate car titles with assertions.
- Modified `GetTestData` to include `carTitle` column.
- Adjusted XPath locator for "Maruti Suzuki" in `NewCarsPage`.
- Updated `TestSpreadSheet.xlsx` to align with new test data.
- Fixed missing closing brace in `BMWCarsPage`.
</commit_message>
<xml_diff>
--- a/resources/TestSpreadSheet.xlsx
+++ b/resources/TestSpreadSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\woodr\source\repos\PageObjectModelPW\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3741B049-5E43-432E-B397-5598FB4E83BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6282C414-A3BD-4E6C-8064-58DEBEB9C23E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{B0960BCF-52F0-4C8D-81B4-BE3083B9D9A2}"/>
+    <workbookView xWindow="0" yWindow="2340" windowWidth="21600" windowHeight="11232" activeTab="1" xr2:uid="{B0960BCF-52F0-4C8D-81B4-BE3083B9D9A2}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginTest" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="34">
   <si>
     <t>username</t>
   </si>
@@ -128,6 +128,18 @@
   </si>
   <si>
     <t>y</t>
+  </si>
+  <si>
+    <t>carTitle</t>
+  </si>
+  <si>
+    <t>BMW Cars</t>
+  </si>
+  <si>
+    <t>Toyota Cars</t>
+  </si>
+  <si>
+    <t>Maruti Cars</t>
   </si>
 </sst>
 </file>
@@ -570,10 +582,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D1C5FD9-9A2A-48E1-96F7-871DE345E001}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -581,7 +593,7 @@
     <col min="2" max="2" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -591,8 +603,11 @@
       <c r="C1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -602,8 +617,11 @@
       <c r="C2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -613,8 +631,11 @@
       <c r="C3" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -623,6 +644,9 @@
       </c>
       <c r="C4" t="s">
         <v>29</v>
+      </c>
+      <c r="D4" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add car name and price test with Excel data source
Introduced CarNameAndPriceTest to automate validation of car names and prices for multiple brands using Playwright and NUnit. Added GetCarNameAndPrices method to CarBase for extracting and printing car details. Updated TestSpreadSheet.xlsx to provide test data, and implemented error handling and resource cleanup in tests.
</commit_message>
<xml_diff>
--- a/resources/TestSpreadSheet.xlsx
+++ b/resources/TestSpreadSheet.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\woodr\source\repos\PageObjectModelPW\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6282C414-A3BD-4E6C-8064-58DEBEB9C23E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA6E3292-34AC-47A9-835C-4A7AA4D46F61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2340" windowWidth="21600" windowHeight="11232" activeTab="1" xr2:uid="{B0960BCF-52F0-4C8D-81B4-BE3083B9D9A2}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{B0960BCF-52F0-4C8D-81B4-BE3083B9D9A2}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginTest" sheetId="1" r:id="rId1"/>
     <sheet name="FindCarTest" sheetId="3" r:id="rId2"/>
-    <sheet name="UserRegTest" sheetId="2" r:id="rId3"/>
+    <sheet name="CarNameAndPrice" sheetId="4" r:id="rId3"/>
+    <sheet name="UserRegTest" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="35">
   <si>
     <t>username</t>
   </si>
@@ -140,6 +141,9 @@
   </si>
   <si>
     <t>Maruti Cars</t>
+  </si>
+  <si>
+    <t>firefox</t>
   </si>
 </sst>
 </file>
@@ -584,13 +588,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D1C5FD9-9A2A-48E1-96F7-871DE345E001}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="14" customWidth="1"/>
+    <col min="4" max="4" width="14.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -655,6 +660,65 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FE1DFB5-BDDC-4489-A51F-779D534F7308}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C10F850C-437A-4316-93AA-6E12EDEC51B3}">
   <dimension ref="A1:B6"/>
   <sheetViews>

</xml_diff>

<commit_message>
Add NUnit categories to tests; update spreadsheet file
Added "SmokeTest" and "BVT" categories to CarNameAndPriceTest.cs and FindNewCarsTest.cs for improved test filtering and organization. Modified TestSpreadSheet.xlsx with new binary changes.
</commit_message>
<xml_diff>
--- a/resources/TestSpreadSheet.xlsx
+++ b/resources/TestSpreadSheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\woodr\source\repos\PageObjectModelPW\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA6E3292-34AC-47A9-835C-4A7AA4D46F61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5913800-3F64-4576-9353-B07C9E1F8685}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{B0960BCF-52F0-4C8D-81B4-BE3083B9D9A2}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="34">
   <si>
     <t>username</t>
   </si>
@@ -141,9 +141,6 @@
   </si>
   <si>
     <t>Maruti Cars</t>
-  </si>
-  <si>
-    <t>firefox</t>
   </si>
 </sst>
 </file>
@@ -664,7 +661,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -696,7 +693,7 @@
         <v>27</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="C3" t="s">
         <v>29</v>

</xml_diff>

<commit_message>
Update new cars flow, locators, and test reliability
- Changed HomePage FindNewCars to use Click instead of MouseOver
- Updated "newcars" locator to match new HTML structure
- Added [Retry(1)] to key test classes for improved reliability
- Changed FindNewCarsTest category to "My Test"
- Updated TestSpreadSheet.xlsx with new test data
</commit_message>
<xml_diff>
--- a/resources/TestSpreadSheet.xlsx
+++ b/resources/TestSpreadSheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\woodr\source\repos\PageObjectModelPW\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5913800-3F64-4576-9353-B07C9E1F8685}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DEE755A-234C-4C0E-A97B-548FAD7EEA89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{B0960BCF-52F0-4C8D-81B4-BE3083B9D9A2}"/>
   </bookViews>
@@ -661,7 +661,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Increase test retry count and improve attempt tracking
Increased the retry count for key tests from 1 to 2. Added per-test attempt tracking using a thread-safe dictionary, logging attempt numbers in reports and screenshot filenames to aid debugging. Updated screenshot naming to prevent overwrites on retries. Commented out a redundant Task.Delay in FindNewCarsTest. Modified TestSpreadSheet.xlsx (details not shown).
</commit_message>
<xml_diff>
--- a/resources/TestSpreadSheet.xlsx
+++ b/resources/TestSpreadSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\woodr\source\repos\PageObjectModelPW\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DEE755A-234C-4C0E-A97B-548FAD7EEA89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1319482-4E4A-4DC2-8728-D08BA60E7163}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{B0960BCF-52F0-4C8D-81B4-BE3083B9D9A2}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{B0960BCF-52F0-4C8D-81B4-BE3083B9D9A2}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginTest" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="35">
   <si>
     <t>username</t>
   </si>
@@ -141,6 +141,9 @@
   </si>
   <si>
     <t>Maruti Cars</t>
+  </si>
+  <si>
+    <t>n</t>
   </si>
 </sst>
 </file>
@@ -585,8 +588,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D1C5FD9-9A2A-48E1-96F7-871DE345E001}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -631,7 +634,7 @@
         <v>25</v>
       </c>
       <c r="C3" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="D3" t="s">
         <v>33</v>
@@ -660,8 +663,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FE1DFB5-BDDC-4489-A51F-779D534F7308}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -696,7 +699,7 @@
         <v>25</v>
       </c>
       <c r="C3" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>